<commit_message>
Added support for 'date needed' field. Updated template.
</commit_message>
<xml_diff>
--- a/Purchase Request Form.xlsx
+++ b/Purchase Request Form.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mg131\Documents\P-Card Folder\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="820" yWindow="720" windowWidth="21580" windowHeight="12260"/>
   </bookViews>
   <sheets>
     <sheet name="DPO BLANK FORM" sheetId="3" r:id="rId1"/>
     <sheet name="ATTACHMENT SHEET" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>GEORGIA INSTITUTE OF TECHNOLOGY</t>
   </si>
@@ -155,6 +155,30 @@
   </si>
   <si>
     <t>XXXX XXXX XXXX 7653</t>
+  </si>
+  <si>
+    <t>Katie Young</t>
+  </si>
+  <si>
+    <t>katie.young@gatech.edu</t>
+  </si>
+  <si>
+    <t>(512) 963-4564</t>
+  </si>
+  <si>
+    <t>Petit Institute for Bioengineering and Bioscience (IBB)</t>
+  </si>
+  <si>
+    <t>315 Ferst Dr. NW</t>
+  </si>
+  <si>
+    <t>Atlanta, GA 30332-0363</t>
+  </si>
+  <si>
+    <t>Todd Sulchek</t>
+  </si>
+  <si>
+    <t>(650) 954-4592</t>
   </si>
 </sst>
 </file>
@@ -168,7 +192,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Geneva"/>
@@ -574,7 +598,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -642,21 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1032,6 +1041,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1153,7 +1171,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
             <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
@@ -1296,7 +1314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1331,7 +1349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1575,16 +1593,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:Y110"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="AA51" sqref="AA51:AA52"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="3.5703125" customWidth="1"/>
@@ -1601,12 +1619,12 @@
     <col min="25" max="25" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75">
+    <row r="1" spans="2:22" ht="15">
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="L1" s="39"/>
+      <c r="L1" s="34"/>
       <c r="O1" s="9"/>
     </row>
     <row r="2" spans="2:22">
@@ -1634,7 +1652,7 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="41" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="1"/>
@@ -1645,116 +1663,118 @@
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="2:22">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="1"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:22">
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:22">
-      <c r="B8" s="41"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="O8" s="129"/>
-      <c r="P8" s="130"/>
-      <c r="Q8" s="130"/>
-      <c r="R8" s="130"/>
-      <c r="S8" s="130"/>
-      <c r="T8" s="130"/>
-      <c r="U8" s="130"/>
-      <c r="V8" s="131"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="O8" s="124"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="126"/>
     </row>
     <row r="9" spans="2:22" ht="3.75" customHeight="1">
-      <c r="B9" s="41"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="O9" s="132"/>
-      <c r="P9" s="133"/>
-      <c r="Q9" s="133"/>
-      <c r="R9" s="133"/>
-      <c r="S9" s="133"/>
-      <c r="T9" s="133"/>
-      <c r="U9" s="133"/>
-      <c r="V9" s="134"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="O9" s="127"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="128"/>
+      <c r="R9" s="128"/>
+      <c r="S9" s="128"/>
+      <c r="T9" s="128"/>
+      <c r="U9" s="128"/>
+      <c r="V9" s="129"/>
     </row>
     <row r="10" spans="2:22" ht="19.5" customHeight="1">
-      <c r="B10" s="41"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
       <c r="L10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="O10" s="136" t="s">
+      <c r="O10" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="P10" s="136"/>
-      <c r="Q10" s="136"/>
-      <c r="R10" s="136"/>
-      <c r="S10" s="136"/>
-      <c r="T10" s="136"/>
-      <c r="U10" s="136"/>
-      <c r="V10" s="136"/>
+      <c r="P10" s="131"/>
+      <c r="Q10" s="131"/>
+      <c r="R10" s="131"/>
+      <c r="S10" s="131"/>
+      <c r="T10" s="131"/>
+      <c r="U10" s="131"/>
+      <c r="V10" s="131"/>
     </row>
     <row r="11" spans="2:22">
-      <c r="B11" s="41"/>
-      <c r="C11" s="73" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="139"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="140"/>
-      <c r="K11" s="141"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="136"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:22">
       <c r="C12" s="2"/>
       <c r="L12" s="10"/>
-      <c r="N12" s="42" t="s">
+      <c r="N12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="O12" s="135"/>
-      <c r="P12" s="135"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="135"/>
-      <c r="S12" s="135"/>
-      <c r="T12" s="135"/>
-      <c r="U12" s="135"/>
-      <c r="V12" s="135"/>
+      <c r="O12" s="130" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="130"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="130"/>
+      <c r="U12" s="130"/>
+      <c r="V12" s="130"/>
     </row>
     <row r="13" spans="2:22">
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="75" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="32"/>
@@ -1765,80 +1785,88 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="102" t="s">
+      <c r="L13" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="103"/>
-      <c r="N13" s="103"/>
-      <c r="O13" s="108"/>
-      <c r="P13" s="109"/>
-      <c r="Q13" s="109"/>
-      <c r="R13" s="109"/>
-      <c r="S13" s="109"/>
-      <c r="T13" s="109"/>
-      <c r="U13" s="109"/>
-      <c r="V13" s="109"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
+      <c r="U13" s="104"/>
+      <c r="V13" s="104"/>
     </row>
     <row r="14" spans="2:22">
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="101"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="95"/>
+      <c r="K14" s="96"/>
       <c r="L14" s="10"/>
-      <c r="N14" s="42" t="s">
+      <c r="N14" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="135"/>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="135"/>
-      <c r="S14" s="135"/>
-      <c r="T14" s="135"/>
-      <c r="U14" s="135"/>
-      <c r="V14" s="135"/>
+      <c r="O14" s="130" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="130"/>
+      <c r="V14" s="130"/>
     </row>
     <row r="15" spans="2:22">
       <c r="B15" s="13"/>
       <c r="K15" s="4"/>
       <c r="L15" s="10"/>
-      <c r="N15" s="71" t="s">
+      <c r="N15" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="114"/>
-      <c r="P15" s="114"/>
-      <c r="Q15" s="114"/>
-      <c r="R15" s="114"/>
-      <c r="S15" s="114"/>
-      <c r="T15" s="114"/>
-      <c r="U15" s="114"/>
-      <c r="V15" s="114"/>
+      <c r="O15" s="109" t="s">
+        <v>48</v>
+      </c>
+      <c r="P15" s="109"/>
+      <c r="Q15" s="109"/>
+      <c r="R15" s="109"/>
+      <c r="S15" s="109"/>
+      <c r="T15" s="109"/>
+      <c r="U15" s="109"/>
+      <c r="V15" s="109"/>
     </row>
     <row r="16" spans="2:22" ht="12" customHeight="1">
-      <c r="B16" s="99"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="101"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="114"/>
-      <c r="P16" s="114"/>
-      <c r="Q16" s="114"/>
-      <c r="R16" s="114"/>
-      <c r="S16" s="114"/>
-      <c r="T16" s="114"/>
-      <c r="U16" s="114"/>
-      <c r="V16" s="114"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="96"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="109"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="109"/>
+      <c r="S16" s="109"/>
+      <c r="T16" s="109"/>
+      <c r="U16" s="109"/>
+      <c r="V16" s="109"/>
     </row>
     <row r="17" spans="2:22" ht="12.75" customHeight="1">
       <c r="B17" s="12"/>
@@ -1851,27 +1879,29 @@
       <c r="I17" s="18"/>
       <c r="J17" s="11"/>
       <c r="K17" s="19"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="114"/>
-      <c r="P17" s="114"/>
-      <c r="Q17" s="114"/>
-      <c r="R17" s="114"/>
-      <c r="S17" s="114"/>
-      <c r="T17" s="114"/>
-      <c r="U17" s="114"/>
-      <c r="V17" s="114"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="P17" s="109"/>
+      <c r="Q17" s="109"/>
+      <c r="R17" s="109"/>
+      <c r="S17" s="109"/>
+      <c r="T17" s="109"/>
+      <c r="U17" s="109"/>
+      <c r="V17" s="109"/>
     </row>
     <row r="18" spans="2:22" ht="12.75" customHeight="1">
-      <c r="B18" s="99"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="101"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="96"/>
       <c r="N18" s="10"/>
       <c r="O18" s="9"/>
     </row>
@@ -1884,503 +1914,500 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="2:22" ht="12.75" customHeight="1">
-      <c r="B20" s="143"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="144"/>
-      <c r="E20" s="145"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="147"/>
-      <c r="H20" s="147"/>
-      <c r="I20" s="147"/>
-      <c r="J20" s="147"/>
-      <c r="K20" s="148"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="139"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="140"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="142"/>
+      <c r="H20" s="142"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="142"/>
+      <c r="K20" s="143"/>
       <c r="O20" s="9"/>
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="2:22" ht="18" customHeight="1">
-      <c r="B21" s="58"/>
-      <c r="C21" s="44" t="s">
+      <c r="B21" s="53"/>
+      <c r="C21" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="111" t="s">
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="O21" s="113"/>
-      <c r="P21" s="111" t="s">
+      <c r="O21" s="108"/>
+      <c r="P21" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="Q21" s="112"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="111" t="s">
+      <c r="Q21" s="107"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="T21" s="112"/>
-      <c r="U21" s="113"/>
-      <c r="V21" s="58"/>
+      <c r="T21" s="107"/>
+      <c r="U21" s="108"/>
+      <c r="V21" s="53"/>
     </row>
     <row r="22" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="168"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="169"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="169"/>
-      <c r="K22" s="169"/>
-      <c r="L22" s="169"/>
-      <c r="M22" s="170"/>
-      <c r="N22" s="137"/>
-      <c r="O22" s="138"/>
-      <c r="P22" s="115"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="171"/>
-      <c r="T22" s="172"/>
-      <c r="U22" s="173"/>
-      <c r="V22" s="59"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="164"/>
+      <c r="K22" s="164"/>
+      <c r="L22" s="164"/>
+      <c r="M22" s="165"/>
+      <c r="N22" s="132"/>
+      <c r="O22" s="133"/>
+      <c r="P22" s="110"/>
+      <c r="Q22" s="111"/>
+      <c r="R22" s="111"/>
+      <c r="S22" s="166"/>
+      <c r="T22" s="167"/>
+      <c r="U22" s="168"/>
+      <c r="V22" s="54"/>
     </row>
     <row r="23" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="95"/>
-      <c r="K23" s="95"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="85"/>
-      <c r="P23" s="105"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="105"/>
-      <c r="T23" s="106"/>
-      <c r="U23" s="107"/>
-      <c r="V23" s="59"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="100"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="101"/>
+      <c r="S23" s="100"/>
+      <c r="T23" s="101"/>
+      <c r="U23" s="102"/>
+      <c r="V23" s="54"/>
     </row>
     <row r="24" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="96"/>
-      <c r="N24" s="84"/>
-      <c r="O24" s="85"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="110"/>
-      <c r="R24" s="106"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="106"/>
-      <c r="U24" s="107"/>
-      <c r="V24" s="59"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="100"/>
+      <c r="Q24" s="105"/>
+      <c r="R24" s="101"/>
+      <c r="S24" s="100"/>
+      <c r="T24" s="101"/>
+      <c r="U24" s="102"/>
+      <c r="V24" s="54"/>
     </row>
     <row r="25" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="96"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="85"/>
-      <c r="P25" s="105"/>
-      <c r="Q25" s="110"/>
-      <c r="R25" s="106"/>
-      <c r="S25" s="105"/>
-      <c r="T25" s="106"/>
-      <c r="U25" s="107"/>
-      <c r="V25" s="59"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="100"/>
+      <c r="Q25" s="105"/>
+      <c r="R25" s="101"/>
+      <c r="S25" s="100"/>
+      <c r="T25" s="101"/>
+      <c r="U25" s="102"/>
+      <c r="V25" s="54"/>
     </row>
     <row r="26" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="95"/>
-      <c r="L26" s="95"/>
-      <c r="M26" s="96"/>
-      <c r="N26" s="84"/>
-      <c r="O26" s="85"/>
-      <c r="P26" s="105"/>
-      <c r="Q26" s="110"/>
-      <c r="R26" s="106"/>
-      <c r="S26" s="105"/>
-      <c r="T26" s="106"/>
-      <c r="U26" s="107"/>
-      <c r="V26" s="59"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="91"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="100"/>
+      <c r="Q26" s="105"/>
+      <c r="R26" s="101"/>
+      <c r="S26" s="100"/>
+      <c r="T26" s="101"/>
+      <c r="U26" s="102"/>
+      <c r="V26" s="54"/>
     </row>
     <row r="27" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="96"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="85"/>
-      <c r="P27" s="105"/>
-      <c r="Q27" s="110"/>
-      <c r="R27" s="106"/>
-      <c r="S27" s="105"/>
-      <c r="T27" s="106"/>
-      <c r="U27" s="107"/>
-      <c r="V27" s="59"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="105"/>
+      <c r="R27" s="101"/>
+      <c r="S27" s="100"/>
+      <c r="T27" s="101"/>
+      <c r="U27" s="102"/>
+      <c r="V27" s="54"/>
     </row>
     <row r="28" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="84"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="105"/>
-      <c r="Q28" s="110"/>
-      <c r="R28" s="106"/>
-      <c r="S28" s="105"/>
-      <c r="T28" s="106"/>
-      <c r="U28" s="107"/>
-      <c r="V28" s="59"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="80"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="101"/>
+      <c r="S28" s="100"/>
+      <c r="T28" s="101"/>
+      <c r="U28" s="102"/>
+      <c r="V28" s="54"/>
     </row>
     <row r="29" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="95"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="84"/>
-      <c r="O29" s="85"/>
-      <c r="P29" s="105"/>
-      <c r="Q29" s="110"/>
-      <c r="R29" s="106"/>
-      <c r="S29" s="105"/>
-      <c r="T29" s="106"/>
-      <c r="U29" s="107"/>
-      <c r="V29" s="59"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="101"/>
+      <c r="S29" s="100"/>
+      <c r="T29" s="101"/>
+      <c r="U29" s="102"/>
+      <c r="V29" s="54"/>
     </row>
     <row r="30" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="95"/>
-      <c r="M30" s="96"/>
-      <c r="N30" s="84"/>
-      <c r="O30" s="85"/>
-      <c r="P30" s="105"/>
-      <c r="Q30" s="110"/>
-      <c r="R30" s="106"/>
-      <c r="S30" s="105"/>
-      <c r="T30" s="106"/>
-      <c r="U30" s="107"/>
-      <c r="V30" s="59"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="105"/>
+      <c r="R30" s="101"/>
+      <c r="S30" s="100"/>
+      <c r="T30" s="101"/>
+      <c r="U30" s="102"/>
+      <c r="V30" s="54"/>
     </row>
     <row r="31" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B31" s="60"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="35"/>
-      <c r="S31" s="105"/>
-      <c r="T31" s="106"/>
-      <c r="U31" s="107"/>
-      <c r="V31" s="59"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="90"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="80"/>
+      <c r="P31" s="202"/>
+      <c r="Q31" s="203"/>
+      <c r="R31" s="204"/>
+      <c r="S31" s="100"/>
+      <c r="T31" s="101"/>
+      <c r="U31" s="102"/>
+      <c r="V31" s="54"/>
     </row>
     <row r="32" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B32" s="60"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="95"/>
-      <c r="M32" s="96"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="105"/>
-      <c r="T32" s="106"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="59"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="202"/>
+      <c r="Q32" s="203"/>
+      <c r="R32" s="204"/>
+      <c r="S32" s="100"/>
+      <c r="T32" s="101"/>
+      <c r="U32" s="102"/>
+      <c r="V32" s="54"/>
     </row>
     <row r="33" spans="2:25" ht="18.75" customHeight="1">
-      <c r="B33" s="60"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95"/>
-      <c r="L33" s="95"/>
-      <c r="M33" s="96"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="105"/>
-      <c r="T33" s="106"/>
-      <c r="U33" s="107"/>
-      <c r="V33" s="59"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="202"/>
+      <c r="Q33" s="203"/>
+      <c r="R33" s="204"/>
+      <c r="S33" s="100"/>
+      <c r="T33" s="101"/>
+      <c r="U33" s="102"/>
+      <c r="V33" s="54"/>
     </row>
     <row r="34" spans="2:25" ht="18.75" customHeight="1">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="95"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="96"/>
-      <c r="N34" s="84"/>
-      <c r="O34" s="85"/>
-      <c r="P34" s="105"/>
-      <c r="Q34" s="110"/>
-      <c r="R34" s="106"/>
-      <c r="S34" s="105"/>
-      <c r="T34" s="106"/>
-      <c r="U34" s="107"/>
-      <c r="V34" s="59"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="100"/>
+      <c r="Q34" s="105"/>
+      <c r="R34" s="101"/>
+      <c r="S34" s="100"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="102"/>
+      <c r="V34" s="54"/>
     </row>
     <row r="35" spans="2:25" ht="18.75" customHeight="1">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="84"/>
-      <c r="O35" s="85"/>
-      <c r="P35" s="105"/>
-      <c r="Q35" s="110"/>
-      <c r="R35" s="106"/>
-      <c r="S35" s="105"/>
-      <c r="T35" s="106"/>
-      <c r="U35" s="107"/>
-      <c r="V35" s="59"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="105"/>
+      <c r="R35" s="101"/>
+      <c r="S35" s="100"/>
+      <c r="T35" s="101"/>
+      <c r="U35" s="102"/>
+      <c r="V35" s="54"/>
     </row>
     <row r="36" spans="2:25" ht="18.75" customHeight="1">
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="174" t="s">
+      <c r="C36" s="35"/>
+      <c r="D36" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="175"/>
-      <c r="F36" s="175"/>
-      <c r="G36" s="175"/>
-      <c r="H36" s="175"/>
-      <c r="I36" s="175"/>
-      <c r="J36" s="175"/>
-      <c r="K36" s="175"/>
-      <c r="L36" s="175"/>
-      <c r="M36" s="176"/>
-      <c r="N36" s="82"/>
-      <c r="O36" s="83"/>
-      <c r="P36" s="153"/>
-      <c r="Q36" s="154"/>
-      <c r="R36" s="155"/>
-      <c r="S36" s="153">
-        <f t="shared" ref="S36" si="0">N36*P36</f>
-        <v>0</v>
-      </c>
-      <c r="T36" s="154"/>
-      <c r="U36" s="155"/>
-      <c r="V36" s="59"/>
+      <c r="E36" s="170"/>
+      <c r="F36" s="170"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="170"/>
+      <c r="I36" s="170"/>
+      <c r="J36" s="170"/>
+      <c r="K36" s="170"/>
+      <c r="L36" s="170"/>
+      <c r="M36" s="171"/>
+      <c r="N36" s="77"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="148"/>
+      <c r="Q36" s="149"/>
+      <c r="R36" s="150"/>
+      <c r="S36" s="148"/>
+      <c r="T36" s="149"/>
+      <c r="U36" s="150"/>
+      <c r="V36" s="54"/>
     </row>
     <row r="37" spans="2:25" ht="15" customHeight="1">
-      <c r="B37" s="177" t="s">
+      <c r="B37" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="178"/>
-      <c r="D37" s="178"/>
-      <c r="E37" s="179"/>
-      <c r="F37" s="66"/>
+      <c r="C37" s="173"/>
+      <c r="D37" s="173"/>
+      <c r="E37" s="174"/>
+      <c r="F37" s="61"/>
       <c r="G37" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="65"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="15" t="s">
         <v>5</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="180" t="s">
+      <c r="L37" s="175" t="s">
         <v>19</v>
       </c>
-      <c r="M37" s="181"/>
-      <c r="N37" s="86"/>
-      <c r="O37" s="87"/>
-      <c r="P37" s="87"/>
-      <c r="Q37" s="87"/>
-      <c r="R37" s="87"/>
-      <c r="S37" s="88"/>
-      <c r="T37" s="149"/>
-      <c r="U37" s="150"/>
-      <c r="V37" s="151"/>
+      <c r="M37" s="176"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="82"/>
+      <c r="R37" s="82"/>
+      <c r="S37" s="83"/>
+      <c r="T37" s="144"/>
+      <c r="U37" s="145"/>
+      <c r="V37" s="146"/>
     </row>
     <row r="38" spans="2:25" s="14" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B38" s="62"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63" t="s">
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="68" t="s">
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="63" t="s">
         <v>6</v>
       </c>
       <c r="R38" s="15"/>
-      <c r="S38" s="156">
+      <c r="S38" s="151">
         <f>SUM(S22:S36)</f>
         <v>0</v>
       </c>
-      <c r="T38" s="157"/>
-      <c r="U38" s="158"/>
+      <c r="T38" s="152"/>
+      <c r="U38" s="153"/>
     </row>
     <row r="39" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B39" s="69"/>
+      <c r="B39" s="64"/>
       <c r="M39" s="5"/>
     </row>
     <row r="40" spans="2:25" s="9" customFormat="1">
-      <c r="B40" s="47"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="49"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="44"/>
       <c r="N40"/>
       <c r="O40"/>
       <c r="P40"/>
@@ -2392,124 +2419,128 @@
       <c r="V40"/>
     </row>
     <row r="41" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B41" s="182" t="s">
+      <c r="B41" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="183"/>
-      <c r="D41" s="184"/>
-      <c r="E41" s="161"/>
-      <c r="F41" s="161"/>
-      <c r="G41" s="161"/>
-      <c r="H41" s="161"/>
-      <c r="I41" s="161"/>
-      <c r="J41" s="161"/>
-      <c r="K41" s="161"/>
-      <c r="L41" s="161"/>
-      <c r="M41" s="161"/>
+      <c r="C41" s="178"/>
+      <c r="D41" s="179"/>
+      <c r="E41" s="156" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="156"/>
+      <c r="G41" s="156"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="156"/>
+      <c r="J41" s="156"/>
+      <c r="K41" s="156"/>
+      <c r="L41" s="156"/>
+      <c r="M41" s="156"/>
       <c r="N41"/>
       <c r="O41"/>
-      <c r="P41" s="185" t="s">
+      <c r="P41" s="180" t="s">
         <v>33</v>
       </c>
-      <c r="Q41" s="186"/>
-      <c r="R41" s="186"/>
-      <c r="S41" s="187"/>
-      <c r="T41" s="162" t="s">
+      <c r="Q41" s="181"/>
+      <c r="R41" s="181"/>
+      <c r="S41" s="182"/>
+      <c r="T41" s="157" t="s">
         <v>22</v>
       </c>
-      <c r="U41" s="163"/>
-      <c r="V41" s="163"/>
-      <c r="W41" s="163"/>
-      <c r="X41" s="163"/>
-      <c r="Y41" s="164"/>
+      <c r="U41" s="158"/>
+      <c r="V41" s="158"/>
+      <c r="W41" s="158"/>
+      <c r="X41" s="158"/>
+      <c r="Y41" s="159"/>
     </row>
     <row r="42" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B42" s="182" t="s">
+      <c r="B42" s="177" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="183"/>
-      <c r="D42" s="184"/>
-      <c r="E42" s="161"/>
-      <c r="F42" s="161"/>
-      <c r="G42" s="161"/>
-      <c r="H42" s="161"/>
-      <c r="I42" s="161"/>
-      <c r="J42" s="161"/>
-      <c r="K42" s="161"/>
-      <c r="L42" s="161"/>
-      <c r="M42" s="161"/>
+      <c r="C42" s="178"/>
+      <c r="D42" s="179"/>
+      <c r="E42" s="156" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="156"/>
+      <c r="G42" s="156"/>
+      <c r="H42" s="156"/>
+      <c r="I42" s="156"/>
+      <c r="J42" s="156"/>
+      <c r="K42" s="156"/>
+      <c r="L42" s="156"/>
+      <c r="M42" s="156"/>
       <c r="N42"/>
       <c r="O42"/>
       <c r="P42"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
-      <c r="T42" s="75" t="s">
+      <c r="T42" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="U42" s="76"/>
-      <c r="V42" s="76"/>
-      <c r="W42" s="76"/>
-      <c r="X42" s="76"/>
-      <c r="Y42" s="77"/>
+      <c r="U42" s="71"/>
+      <c r="V42" s="71"/>
+      <c r="W42" s="71"/>
+      <c r="X42" s="71"/>
+      <c r="Y42" s="72"/>
     </row>
     <row r="43" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="54"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="49"/>
       <c r="N43"/>
       <c r="O43"/>
       <c r="P43"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
-      <c r="T43" s="75" t="s">
+      <c r="T43" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="U43" s="76"/>
-      <c r="V43" s="76"/>
-      <c r="W43" s="76"/>
-      <c r="X43" s="76"/>
-      <c r="Y43" s="77"/>
+      <c r="U43" s="71"/>
+      <c r="V43" s="71"/>
+      <c r="W43" s="71"/>
+      <c r="X43" s="71"/>
+      <c r="Y43" s="72"/>
     </row>
     <row r="44" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B44" s="55"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="64" t="s">
+      <c r="B44" s="50"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="57"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="52"/>
       <c r="N44"/>
       <c r="O44"/>
       <c r="P44"/>
-      <c r="Q44" s="72"/>
-      <c r="R44" s="72"/>
-      <c r="S44" s="72"/>
-      <c r="T44" s="165" t="s">
+      <c r="Q44" s="67"/>
+      <c r="R44" s="67"/>
+      <c r="S44" s="67"/>
+      <c r="T44" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="U44" s="166"/>
-      <c r="V44" s="166"/>
-      <c r="W44" s="166"/>
-      <c r="X44" s="166"/>
-      <c r="Y44" s="167"/>
+      <c r="U44" s="161"/>
+      <c r="V44" s="161"/>
+      <c r="W44" s="161"/>
+      <c r="X44" s="161"/>
+      <c r="Y44" s="162"/>
     </row>
     <row r="45" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B45"/>
@@ -2530,14 +2561,14 @@
       <c r="Q45"/>
       <c r="R45"/>
       <c r="S45"/>
-      <c r="T45" s="93" t="s">
+      <c r="T45" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="U45" s="93"/>
-      <c r="V45" s="93"/>
-      <c r="W45" s="93"/>
-      <c r="X45" s="93"/>
-      <c r="Y45" s="93"/>
+      <c r="U45" s="88"/>
+      <c r="V45" s="88"/>
+      <c r="W45" s="88"/>
+      <c r="X45" s="88"/>
+      <c r="Y45" s="88"/>
     </row>
     <row r="46" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B46"/>
@@ -2558,92 +2589,92 @@
       <c r="Q46"/>
       <c r="R46"/>
       <c r="S46"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="74"/>
-      <c r="W46" s="74"/>
-      <c r="X46" s="74"/>
-      <c r="Y46" s="74"/>
+      <c r="T46" s="69"/>
+      <c r="U46" s="69"/>
+      <c r="V46" s="69"/>
+      <c r="W46" s="69"/>
+      <c r="X46" s="69"/>
+      <c r="Y46" s="69"/>
     </row>
     <row r="47" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B47" s="160" t="s">
+      <c r="B47" s="155" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="160"/>
-      <c r="D47" s="160"/>
-      <c r="E47" s="147"/>
-      <c r="F47" s="147"/>
-      <c r="G47" s="147"/>
-      <c r="H47" s="147"/>
-      <c r="I47" s="147"/>
-      <c r="J47" s="147"/>
-      <c r="K47" s="147"/>
-      <c r="L47" s="147"/>
-      <c r="M47" s="147"/>
-      <c r="N47" s="147"/>
-      <c r="O47" s="147"/>
-      <c r="P47" s="147"/>
-      <c r="Q47" s="147"/>
-      <c r="R47" s="147"/>
-      <c r="S47" s="147"/>
-      <c r="T47" s="147"/>
-      <c r="U47" s="147"/>
-      <c r="V47" s="147"/>
-      <c r="W47" s="41"/>
-      <c r="X47" s="74"/>
-      <c r="Y47" s="74"/>
+      <c r="C47" s="155"/>
+      <c r="D47" s="155"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="142"/>
+      <c r="G47" s="142"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="142"/>
+      <c r="J47" s="142"/>
+      <c r="K47" s="142"/>
+      <c r="L47" s="142"/>
+      <c r="M47" s="142"/>
+      <c r="N47" s="142"/>
+      <c r="O47" s="142"/>
+      <c r="P47" s="142"/>
+      <c r="Q47" s="142"/>
+      <c r="R47" s="142"/>
+      <c r="S47" s="142"/>
+      <c r="T47" s="142"/>
+      <c r="U47" s="142"/>
+      <c r="V47" s="142"/>
+      <c r="W47" s="36"/>
+      <c r="X47" s="69"/>
+      <c r="Y47" s="69"/>
     </row>
     <row r="48" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="89"/>
-      <c r="J48" s="89"/>
-      <c r="K48" s="89"/>
-      <c r="L48" s="89"/>
-      <c r="M48" s="89"/>
-      <c r="N48" s="89"/>
-      <c r="O48" s="89"/>
-      <c r="P48" s="89"/>
-      <c r="Q48" s="89"/>
-      <c r="R48" s="89"/>
-      <c r="S48" s="89"/>
-      <c r="T48" s="89"/>
-      <c r="U48" s="89"/>
-      <c r="V48" s="89"/>
-      <c r="W48" s="74"/>
-      <c r="X48" s="74"/>
-      <c r="Y48" s="74"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="84"/>
+      <c r="I48" s="84"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="84"/>
+      <c r="L48" s="84"/>
+      <c r="M48" s="84"/>
+      <c r="N48" s="84"/>
+      <c r="O48" s="84"/>
+      <c r="P48" s="84"/>
+      <c r="Q48" s="84"/>
+      <c r="R48" s="84"/>
+      <c r="S48" s="84"/>
+      <c r="T48" s="84"/>
+      <c r="U48" s="84"/>
+      <c r="V48" s="84"/>
+      <c r="W48" s="69"/>
+      <c r="X48" s="69"/>
+      <c r="Y48" s="69"/>
     </row>
     <row r="49" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="89"/>
-      <c r="K49" s="89"/>
-      <c r="L49" s="89"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="89"/>
-      <c r="O49" s="89"/>
-      <c r="P49" s="89"/>
-      <c r="Q49" s="89"/>
-      <c r="R49" s="89"/>
-      <c r="S49" s="89"/>
-      <c r="T49" s="89"/>
-      <c r="U49" s="89"/>
-      <c r="V49" s="89"/>
-      <c r="W49" s="74"/>
-      <c r="X49" s="74"/>
-      <c r="Y49" s="74"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="84"/>
+      <c r="I49" s="84"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="84"/>
+      <c r="L49" s="84"/>
+      <c r="M49" s="84"/>
+      <c r="N49" s="84"/>
+      <c r="O49" s="84"/>
+      <c r="P49" s="84"/>
+      <c r="Q49" s="84"/>
+      <c r="R49" s="84"/>
+      <c r="S49" s="84"/>
+      <c r="T49" s="84"/>
+      <c r="U49" s="84"/>
+      <c r="V49" s="84"/>
+      <c r="W49" s="69"/>
+      <c r="X49" s="69"/>
+      <c r="Y49" s="69"/>
     </row>
     <row r="50" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B50"/>
@@ -2678,47 +2709,47 @@
       <c r="O51"/>
     </row>
     <row r="52" spans="2:25" s="9" customFormat="1">
-      <c r="B52" s="122" t="s">
+      <c r="B52" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="123"/>
-      <c r="D52" s="124" t="s">
+      <c r="C52" s="118"/>
+      <c r="D52" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="125"/>
-      <c r="F52" s="126"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="121"/>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
       <c r="L52"/>
-      <c r="M52" s="90" t="s">
+      <c r="M52" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="N52" s="91"/>
-      <c r="O52" s="91"/>
-      <c r="P52" s="91"/>
-      <c r="Q52" s="91"/>
-      <c r="R52" s="91"/>
-      <c r="S52" s="91"/>
-      <c r="T52" s="91"/>
-      <c r="U52" s="91"/>
-      <c r="V52" s="92"/>
+      <c r="N52" s="86"/>
+      <c r="O52" s="86"/>
+      <c r="P52" s="86"/>
+      <c r="Q52" s="86"/>
+      <c r="R52" s="86"/>
+      <c r="S52" s="86"/>
+      <c r="T52" s="86"/>
+      <c r="U52" s="86"/>
+      <c r="V52" s="87"/>
     </row>
     <row r="53" spans="2:25" s="16" customFormat="1">
-      <c r="B53" s="119"/>
-      <c r="C53" s="119"/>
-      <c r="D53" s="127"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="128"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="114"/>
+      <c r="D53" s="122"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
       <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
-      <c r="M53" s="67"/>
+      <c r="M53" s="62"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -2730,72 +2761,72 @@
       <c r="V53" s="4"/>
     </row>
     <row r="54" spans="2:25" s="16" customFormat="1">
-      <c r="B54" s="120"/>
-      <c r="C54" s="121"/>
-      <c r="D54" s="117"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="116"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="113"/>
+      <c r="F54" s="113"/>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
       <c r="L54"/>
-      <c r="M54" s="152" t="s">
+      <c r="M54" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="N54" s="103"/>
-      <c r="O54" s="81" t="s">
+      <c r="N54" s="98"/>
+      <c r="O54" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="P54" s="81"/>
-      <c r="Q54" s="81"/>
-      <c r="R54" s="81"/>
-      <c r="S54" s="81"/>
-      <c r="T54" s="81"/>
-      <c r="U54" s="81"/>
-      <c r="V54" s="159"/>
+      <c r="P54" s="76"/>
+      <c r="Q54" s="76"/>
+      <c r="R54" s="76"/>
+      <c r="S54" s="76"/>
+      <c r="T54" s="76"/>
+      <c r="U54" s="76"/>
+      <c r="V54" s="154"/>
     </row>
     <row r="55" spans="2:25" s="16" customFormat="1">
-      <c r="B55" s="120"/>
-      <c r="C55" s="121"/>
-      <c r="D55" s="117"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="113"/>
+      <c r="F55" s="113"/>
       <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
-      <c r="M55" s="152" t="s">
+      <c r="M55" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="N55" s="103"/>
-      <c r="O55" s="81" t="s">
+      <c r="N55" s="98"/>
+      <c r="O55" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="P55" s="81"/>
-      <c r="Q55" s="81"/>
-      <c r="R55" s="81"/>
-      <c r="S55" s="81"/>
+      <c r="P55" s="76"/>
+      <c r="Q55" s="76"/>
+      <c r="R55" s="76"/>
+      <c r="S55" s="76"/>
       <c r="T55"/>
       <c r="U55"/>
       <c r="V55" s="4"/>
     </row>
     <row r="56" spans="2:25" s="16" customFormat="1">
-      <c r="B56" s="120"/>
-      <c r="C56" s="121"/>
-      <c r="D56" s="117"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="118"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="116"/>
+      <c r="D56" s="112"/>
+      <c r="E56" s="113"/>
+      <c r="F56" s="113"/>
       <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56"/>
-      <c r="M56" s="67"/>
+      <c r="M56" s="62"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -2807,29 +2838,29 @@
       <c r="V56" s="4"/>
     </row>
     <row r="57" spans="2:25" s="16" customFormat="1">
-      <c r="B57" s="120"/>
-      <c r="C57" s="121"/>
-      <c r="D57" s="117"/>
-      <c r="E57" s="118"/>
-      <c r="F57" s="118"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="116"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="113"/>
+      <c r="F57" s="113"/>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
-      <c r="M57" s="149" t="s">
+      <c r="M57" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="N57" s="150"/>
-      <c r="O57" s="150"/>
-      <c r="P57" s="150"/>
-      <c r="Q57" s="150"/>
-      <c r="R57" s="150"/>
-      <c r="S57" s="150"/>
-      <c r="T57" s="150"/>
-      <c r="U57" s="150"/>
-      <c r="V57" s="151"/>
+      <c r="N57" s="145"/>
+      <c r="O57" s="145"/>
+      <c r="P57" s="145"/>
+      <c r="Q57" s="145"/>
+      <c r="R57" s="145"/>
+      <c r="S57" s="145"/>
+      <c r="T57" s="145"/>
+      <c r="U57" s="145"/>
+      <c r="V57" s="146"/>
     </row>
     <row r="58" spans="2:25" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="B58"/>
@@ -2894,28 +2925,28 @@
       <c r="U60" s="20"/>
       <c r="V60" s="20"/>
     </row>
-    <row r="61" spans="2:25" s="9" customFormat="1" ht="11.25">
-      <c r="B61" s="142"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="142"/>
-      <c r="E61" s="142"/>
-      <c r="F61" s="142"/>
-      <c r="G61" s="142"/>
-      <c r="H61" s="142"/>
-      <c r="I61" s="142"/>
-      <c r="J61" s="142"/>
-      <c r="K61" s="142"/>
-      <c r="L61" s="142"/>
-      <c r="M61" s="142"/>
-      <c r="N61" s="142"/>
-      <c r="O61" s="142"/>
-      <c r="P61" s="142"/>
-      <c r="Q61" s="142"/>
-      <c r="R61" s="142"/>
-      <c r="S61" s="142"/>
-      <c r="T61" s="142"/>
-      <c r="U61" s="142"/>
-      <c r="V61" s="142"/>
+    <row r="61" spans="2:25" s="9" customFormat="1" ht="11">
+      <c r="B61" s="137"/>
+      <c r="C61" s="137"/>
+      <c r="D61" s="137"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="137"/>
+      <c r="G61" s="137"/>
+      <c r="H61" s="137"/>
+      <c r="I61" s="137"/>
+      <c r="J61" s="137"/>
+      <c r="K61" s="137"/>
+      <c r="L61" s="137"/>
+      <c r="M61" s="137"/>
+      <c r="N61" s="137"/>
+      <c r="O61" s="137"/>
+      <c r="P61" s="137"/>
+      <c r="Q61" s="137"/>
+      <c r="R61" s="137"/>
+      <c r="S61" s="137"/>
+      <c r="T61" s="137"/>
+      <c r="U61" s="137"/>
+      <c r="V61" s="137"/>
     </row>
     <row r="62" spans="2:25" s="9" customFormat="1">
       <c r="B62"/>
@@ -3093,7 +3124,7 @@
       <c r="V110"/>
     </row>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="116">
     <mergeCell ref="E49:V49"/>
     <mergeCell ref="S26:U26"/>
     <mergeCell ref="D34:M34"/>
@@ -3115,6 +3146,9 @@
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="P41:S41"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="N32:O32"/>
     <mergeCell ref="D21:M21"/>
     <mergeCell ref="P36:R36"/>
     <mergeCell ref="P35:R35"/>
@@ -3134,6 +3168,9 @@
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="P32:R32"/>
     <mergeCell ref="F11:K11"/>
     <mergeCell ref="B61:V61"/>
     <mergeCell ref="B20:E20"/>
@@ -3206,13 +3243,21 @@
     <mergeCell ref="P22:R22"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="O13" r:id="rId1"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.31" header="0.34" footer="0.28000000000000003"/>
-  <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="78" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;6FORM:  ME PCR 2/2003</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3224,7 +3269,7 @@
       <selection activeCell="B6" sqref="B6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="21" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="21" customWidth="1"/>
@@ -3241,36 +3286,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1">
-      <c r="E1" s="191" t="s">
+      <c r="E1" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
       <c r="K1" s="21" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="E2" s="191" t="s">
+      <c r="E2" s="186" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
-      <c r="E3" s="191" t="s">
+      <c r="E3" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="191"/>
-      <c r="G3" s="191"/>
-      <c r="H3" s="191"/>
-      <c r="I3" s="191"/>
+      <c r="F3" s="186"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
       <c r="J3" s="23">
         <f>'DPO BLANK FORM'!O8</f>
         <v>0</v>
@@ -3283,487 +3328,487 @@
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="192" t="s">
+      <c r="B5" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="194"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="188"/>
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="189"/>
       <c r="I5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="198" t="s">
+      <c r="K5" s="193" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="199"/>
-      <c r="M5" s="200"/>
-    </row>
-    <row r="6" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L5" s="194"/>
+      <c r="M5" s="195"/>
+    </row>
+    <row r="6" spans="1:13" ht="23" customHeight="1">
       <c r="A6" s="27"/>
-      <c r="B6" s="195"/>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="197"/>
+      <c r="B6" s="190"/>
+      <c r="C6" s="191"/>
+      <c r="D6" s="191"/>
+      <c r="E6" s="191"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="191"/>
+      <c r="H6" s="192"/>
       <c r="I6" s="28"/>
       <c r="J6" s="29"/>
-      <c r="K6" s="204">
+      <c r="K6" s="199">
         <f>I6*J6</f>
         <v>0</v>
       </c>
-      <c r="L6" s="205"/>
-      <c r="M6" s="206"/>
-    </row>
-    <row r="7" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L6" s="200"/>
+      <c r="M6" s="201"/>
+    </row>
+    <row r="7" spans="1:13" ht="23" customHeight="1">
       <c r="A7" s="27"/>
-      <c r="B7" s="195"/>
-      <c r="C7" s="196"/>
-      <c r="D7" s="196"/>
-      <c r="E7" s="196"/>
-      <c r="F7" s="196"/>
-      <c r="G7" s="196"/>
-      <c r="H7" s="197"/>
+      <c r="B7" s="190"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="192"/>
       <c r="I7" s="28"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="188">
+      <c r="K7" s="183">
         <f t="shared" ref="K7:K30" si="0">I7*J7</f>
         <v>0</v>
       </c>
-      <c r="L7" s="189"/>
-      <c r="M7" s="190"/>
-    </row>
-    <row r="8" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L7" s="184"/>
+      <c r="M7" s="185"/>
+    </row>
+    <row r="8" spans="1:13" ht="23" customHeight="1">
       <c r="A8" s="27"/>
-      <c r="B8" s="195"/>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="197"/>
+      <c r="B8" s="190"/>
+      <c r="C8" s="191"/>
+      <c r="D8" s="191"/>
+      <c r="E8" s="191"/>
+      <c r="F8" s="191"/>
+      <c r="G8" s="191"/>
+      <c r="H8" s="192"/>
       <c r="I8" s="28"/>
       <c r="J8" s="31"/>
-      <c r="K8" s="188">
+      <c r="K8" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8" s="189"/>
-      <c r="M8" s="190"/>
-    </row>
-    <row r="9" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L8" s="184"/>
+      <c r="M8" s="185"/>
+    </row>
+    <row r="9" spans="1:13" ht="23" customHeight="1">
       <c r="A9" s="27"/>
-      <c r="B9" s="195"/>
-      <c r="C9" s="196"/>
-      <c r="D9" s="196"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="197"/>
+      <c r="B9" s="190"/>
+      <c r="C9" s="191"/>
+      <c r="D9" s="191"/>
+      <c r="E9" s="191"/>
+      <c r="F9" s="191"/>
+      <c r="G9" s="191"/>
+      <c r="H9" s="192"/>
       <c r="I9" s="28"/>
       <c r="J9" s="31"/>
-      <c r="K9" s="188">
+      <c r="K9" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L9" s="189"/>
-      <c r="M9" s="190"/>
-    </row>
-    <row r="10" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L9" s="184"/>
+      <c r="M9" s="185"/>
+    </row>
+    <row r="10" spans="1:13" ht="23" customHeight="1">
       <c r="A10" s="27"/>
-      <c r="B10" s="195"/>
-      <c r="C10" s="196"/>
-      <c r="D10" s="196"/>
-      <c r="E10" s="196"/>
-      <c r="F10" s="196"/>
-      <c r="G10" s="196"/>
-      <c r="H10" s="197"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="191"/>
+      <c r="H10" s="192"/>
       <c r="I10" s="28"/>
       <c r="J10" s="31"/>
-      <c r="K10" s="188">
+      <c r="K10" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10" s="189"/>
-      <c r="M10" s="190"/>
-    </row>
-    <row r="11" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L10" s="184"/>
+      <c r="M10" s="185"/>
+    </row>
+    <row r="11" spans="1:13" ht="23" customHeight="1">
       <c r="A11" s="27"/>
-      <c r="B11" s="195"/>
-      <c r="C11" s="196"/>
-      <c r="D11" s="196"/>
-      <c r="E11" s="196"/>
-      <c r="F11" s="196"/>
-      <c r="G11" s="196"/>
-      <c r="H11" s="197"/>
+      <c r="B11" s="190"/>
+      <c r="C11" s="191"/>
+      <c r="D11" s="191"/>
+      <c r="E11" s="191"/>
+      <c r="F11" s="191"/>
+      <c r="G11" s="191"/>
+      <c r="H11" s="192"/>
       <c r="I11" s="28"/>
       <c r="J11" s="31"/>
-      <c r="K11" s="188">
+      <c r="K11" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11" s="189"/>
-      <c r="M11" s="190"/>
-    </row>
-    <row r="12" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L11" s="184"/>
+      <c r="M11" s="185"/>
+    </row>
+    <row r="12" spans="1:13" ht="23" customHeight="1">
       <c r="A12" s="27"/>
-      <c r="B12" s="195"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="196"/>
-      <c r="E12" s="196"/>
-      <c r="F12" s="196"/>
-      <c r="G12" s="196"/>
-      <c r="H12" s="197"/>
+      <c r="B12" s="190"/>
+      <c r="C12" s="191"/>
+      <c r="D12" s="191"/>
+      <c r="E12" s="191"/>
+      <c r="F12" s="191"/>
+      <c r="G12" s="191"/>
+      <c r="H12" s="192"/>
       <c r="I12" s="28"/>
       <c r="J12" s="31"/>
-      <c r="K12" s="188">
+      <c r="K12" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="189"/>
-      <c r="M12" s="190"/>
-    </row>
-    <row r="13" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L12" s="184"/>
+      <c r="M12" s="185"/>
+    </row>
+    <row r="13" spans="1:13" ht="23" customHeight="1">
       <c r="A13" s="27"/>
-      <c r="B13" s="195"/>
-      <c r="C13" s="196"/>
-      <c r="D13" s="196"/>
-      <c r="E13" s="196"/>
-      <c r="F13" s="196"/>
-      <c r="G13" s="196"/>
-      <c r="H13" s="197"/>
+      <c r="B13" s="190"/>
+      <c r="C13" s="191"/>
+      <c r="D13" s="191"/>
+      <c r="E13" s="191"/>
+      <c r="F13" s="191"/>
+      <c r="G13" s="191"/>
+      <c r="H13" s="192"/>
       <c r="I13" s="28"/>
       <c r="J13" s="31"/>
-      <c r="K13" s="188">
+      <c r="K13" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="189"/>
-      <c r="M13" s="190"/>
-    </row>
-    <row r="14" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L13" s="184"/>
+      <c r="M13" s="185"/>
+    </row>
+    <row r="14" spans="1:13" ht="23" customHeight="1">
       <c r="A14" s="27"/>
-      <c r="B14" s="195"/>
-      <c r="C14" s="196"/>
-      <c r="D14" s="196"/>
-      <c r="E14" s="196"/>
-      <c r="F14" s="196"/>
-      <c r="G14" s="196"/>
-      <c r="H14" s="197"/>
+      <c r="B14" s="190"/>
+      <c r="C14" s="191"/>
+      <c r="D14" s="191"/>
+      <c r="E14" s="191"/>
+      <c r="F14" s="191"/>
+      <c r="G14" s="191"/>
+      <c r="H14" s="192"/>
       <c r="I14" s="28"/>
       <c r="J14" s="31"/>
-      <c r="K14" s="188">
+      <c r="K14" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="189"/>
-      <c r="M14" s="190"/>
-    </row>
-    <row r="15" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L14" s="184"/>
+      <c r="M14" s="185"/>
+    </row>
+    <row r="15" spans="1:13" ht="23" customHeight="1">
       <c r="A15" s="27"/>
-      <c r="B15" s="195"/>
-      <c r="C15" s="196"/>
-      <c r="D15" s="196"/>
-      <c r="E15" s="196"/>
-      <c r="F15" s="196"/>
-      <c r="G15" s="196"/>
-      <c r="H15" s="197"/>
+      <c r="B15" s="190"/>
+      <c r="C15" s="191"/>
+      <c r="D15" s="191"/>
+      <c r="E15" s="191"/>
+      <c r="F15" s="191"/>
+      <c r="G15" s="191"/>
+      <c r="H15" s="192"/>
       <c r="I15" s="28"/>
       <c r="J15" s="31"/>
-      <c r="K15" s="188">
+      <c r="K15" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="189"/>
-      <c r="M15" s="190"/>
-    </row>
-    <row r="16" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L15" s="184"/>
+      <c r="M15" s="185"/>
+    </row>
+    <row r="16" spans="1:13" ht="23" customHeight="1">
       <c r="A16" s="27"/>
-      <c r="B16" s="195"/>
-      <c r="C16" s="196"/>
-      <c r="D16" s="196"/>
-      <c r="E16" s="196"/>
-      <c r="F16" s="196"/>
-      <c r="G16" s="196"/>
-      <c r="H16" s="197"/>
+      <c r="B16" s="190"/>
+      <c r="C16" s="191"/>
+      <c r="D16" s="191"/>
+      <c r="E16" s="191"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="191"/>
+      <c r="H16" s="192"/>
       <c r="I16" s="28"/>
       <c r="J16" s="31"/>
-      <c r="K16" s="188">
+      <c r="K16" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16" s="189"/>
-      <c r="M16" s="190"/>
-    </row>
-    <row r="17" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L16" s="184"/>
+      <c r="M16" s="185"/>
+    </row>
+    <row r="17" spans="1:13" ht="23" customHeight="1">
       <c r="A17" s="27"/>
-      <c r="B17" s="195"/>
-      <c r="C17" s="196"/>
-      <c r="D17" s="196"/>
-      <c r="E17" s="196"/>
-      <c r="F17" s="196"/>
-      <c r="G17" s="196"/>
-      <c r="H17" s="197"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="191"/>
+      <c r="D17" s="191"/>
+      <c r="E17" s="191"/>
+      <c r="F17" s="191"/>
+      <c r="G17" s="191"/>
+      <c r="H17" s="192"/>
       <c r="I17" s="28"/>
       <c r="J17" s="31"/>
-      <c r="K17" s="188">
+      <c r="K17" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17" s="189"/>
-      <c r="M17" s="190"/>
-    </row>
-    <row r="18" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L17" s="184"/>
+      <c r="M17" s="185"/>
+    </row>
+    <row r="18" spans="1:13" ht="23" customHeight="1">
       <c r="A18" s="27"/>
-      <c r="B18" s="195"/>
-      <c r="C18" s="196"/>
-      <c r="D18" s="196"/>
-      <c r="E18" s="196"/>
-      <c r="F18" s="196"/>
-      <c r="G18" s="196"/>
-      <c r="H18" s="197"/>
+      <c r="B18" s="190"/>
+      <c r="C18" s="191"/>
+      <c r="D18" s="191"/>
+      <c r="E18" s="191"/>
+      <c r="F18" s="191"/>
+      <c r="G18" s="191"/>
+      <c r="H18" s="192"/>
       <c r="I18" s="28"/>
       <c r="J18" s="31"/>
-      <c r="K18" s="188">
+      <c r="K18" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18" s="189"/>
-      <c r="M18" s="190"/>
-    </row>
-    <row r="19" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L18" s="184"/>
+      <c r="M18" s="185"/>
+    </row>
+    <row r="19" spans="1:13" ht="23" customHeight="1">
       <c r="A19" s="27"/>
-      <c r="B19" s="195"/>
-      <c r="C19" s="196"/>
-      <c r="D19" s="196"/>
-      <c r="E19" s="196"/>
-      <c r="F19" s="196"/>
-      <c r="G19" s="196"/>
-      <c r="H19" s="197"/>
+      <c r="B19" s="190"/>
+      <c r="C19" s="191"/>
+      <c r="D19" s="191"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="192"/>
       <c r="I19" s="28"/>
       <c r="J19" s="31"/>
-      <c r="K19" s="188">
+      <c r="K19" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="189"/>
-      <c r="M19" s="190"/>
-    </row>
-    <row r="20" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L19" s="184"/>
+      <c r="M19" s="185"/>
+    </row>
+    <row r="20" spans="1:13" ht="23" customHeight="1">
       <c r="A20" s="27"/>
-      <c r="B20" s="195"/>
-      <c r="C20" s="196"/>
-      <c r="D20" s="196"/>
-      <c r="E20" s="196"/>
-      <c r="F20" s="196"/>
-      <c r="G20" s="196"/>
-      <c r="H20" s="197"/>
+      <c r="B20" s="190"/>
+      <c r="C20" s="191"/>
+      <c r="D20" s="191"/>
+      <c r="E20" s="191"/>
+      <c r="F20" s="191"/>
+      <c r="G20" s="191"/>
+      <c r="H20" s="192"/>
       <c r="I20" s="28"/>
       <c r="J20" s="31"/>
-      <c r="K20" s="188">
+      <c r="K20" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="189"/>
-      <c r="M20" s="190"/>
-    </row>
-    <row r="21" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L20" s="184"/>
+      <c r="M20" s="185"/>
+    </row>
+    <row r="21" spans="1:13" ht="23" customHeight="1">
       <c r="A21" s="27"/>
-      <c r="B21" s="195"/>
-      <c r="C21" s="196"/>
-      <c r="D21" s="196"/>
-      <c r="E21" s="196"/>
-      <c r="F21" s="196"/>
-      <c r="G21" s="196"/>
-      <c r="H21" s="197"/>
+      <c r="B21" s="190"/>
+      <c r="C21" s="191"/>
+      <c r="D21" s="191"/>
+      <c r="E21" s="191"/>
+      <c r="F21" s="191"/>
+      <c r="G21" s="191"/>
+      <c r="H21" s="192"/>
       <c r="I21" s="28"/>
       <c r="J21" s="31"/>
-      <c r="K21" s="188">
+      <c r="K21" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" s="189"/>
-      <c r="M21" s="190"/>
-    </row>
-    <row r="22" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L21" s="184"/>
+      <c r="M21" s="185"/>
+    </row>
+    <row r="22" spans="1:13" ht="23" customHeight="1">
       <c r="A22" s="27"/>
-      <c r="B22" s="195"/>
-      <c r="C22" s="196"/>
-      <c r="D22" s="196"/>
-      <c r="E22" s="196"/>
-      <c r="F22" s="196"/>
-      <c r="G22" s="196"/>
-      <c r="H22" s="197"/>
+      <c r="B22" s="190"/>
+      <c r="C22" s="191"/>
+      <c r="D22" s="191"/>
+      <c r="E22" s="191"/>
+      <c r="F22" s="191"/>
+      <c r="G22" s="191"/>
+      <c r="H22" s="192"/>
       <c r="I22" s="28"/>
       <c r="J22" s="31"/>
-      <c r="K22" s="188">
+      <c r="K22" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22" s="189"/>
-      <c r="M22" s="190"/>
-    </row>
-    <row r="23" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L22" s="184"/>
+      <c r="M22" s="185"/>
+    </row>
+    <row r="23" spans="1:13" ht="23" customHeight="1">
       <c r="A23" s="27"/>
-      <c r="B23" s="195"/>
-      <c r="C23" s="196"/>
-      <c r="D23" s="196"/>
-      <c r="E23" s="196"/>
-      <c r="F23" s="196"/>
-      <c r="G23" s="196"/>
-      <c r="H23" s="197"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="191"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="191"/>
+      <c r="F23" s="191"/>
+      <c r="G23" s="191"/>
+      <c r="H23" s="192"/>
       <c r="I23" s="28"/>
       <c r="J23" s="31"/>
-      <c r="K23" s="188">
+      <c r="K23" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23" s="189"/>
-      <c r="M23" s="190"/>
-    </row>
-    <row r="24" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L23" s="184"/>
+      <c r="M23" s="185"/>
+    </row>
+    <row r="24" spans="1:13" ht="23" customHeight="1">
       <c r="A24" s="27"/>
-      <c r="B24" s="195"/>
-      <c r="C24" s="196"/>
-      <c r="D24" s="196"/>
-      <c r="E24" s="196"/>
-      <c r="F24" s="196"/>
-      <c r="G24" s="196"/>
-      <c r="H24" s="197"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="191"/>
+      <c r="D24" s="191"/>
+      <c r="E24" s="191"/>
+      <c r="F24" s="191"/>
+      <c r="G24" s="191"/>
+      <c r="H24" s="192"/>
       <c r="I24" s="28"/>
       <c r="J24" s="31"/>
-      <c r="K24" s="188">
+      <c r="K24" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24" s="189"/>
-      <c r="M24" s="190"/>
-    </row>
-    <row r="25" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L24" s="184"/>
+      <c r="M24" s="185"/>
+    </row>
+    <row r="25" spans="1:13" ht="23" customHeight="1">
       <c r="A25" s="27"/>
-      <c r="B25" s="195"/>
-      <c r="C25" s="196"/>
-      <c r="D25" s="196"/>
-      <c r="E25" s="196"/>
-      <c r="F25" s="196"/>
-      <c r="G25" s="196"/>
-      <c r="H25" s="197"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="191"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="191"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="191"/>
+      <c r="H25" s="192"/>
       <c r="I25" s="28"/>
       <c r="J25" s="31"/>
-      <c r="K25" s="188">
+      <c r="K25" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L25" s="189"/>
-      <c r="M25" s="190"/>
-    </row>
-    <row r="26" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L25" s="184"/>
+      <c r="M25" s="185"/>
+    </row>
+    <row r="26" spans="1:13" ht="23" customHeight="1">
       <c r="A26" s="27"/>
-      <c r="B26" s="195"/>
-      <c r="C26" s="196"/>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196"/>
-      <c r="F26" s="196"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="197"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="191"/>
+      <c r="D26" s="191"/>
+      <c r="E26" s="191"/>
+      <c r="F26" s="191"/>
+      <c r="G26" s="191"/>
+      <c r="H26" s="192"/>
       <c r="I26" s="28"/>
       <c r="J26" s="31"/>
-      <c r="K26" s="188">
+      <c r="K26" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L26" s="189"/>
-      <c r="M26" s="190"/>
-    </row>
-    <row r="27" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L26" s="184"/>
+      <c r="M26" s="185"/>
+    </row>
+    <row r="27" spans="1:13" ht="23" customHeight="1">
       <c r="A27" s="27"/>
-      <c r="B27" s="195"/>
-      <c r="C27" s="196"/>
-      <c r="D27" s="196"/>
-      <c r="E27" s="196"/>
-      <c r="F27" s="196"/>
-      <c r="G27" s="196"/>
-      <c r="H27" s="197"/>
+      <c r="B27" s="190"/>
+      <c r="C27" s="191"/>
+      <c r="D27" s="191"/>
+      <c r="E27" s="191"/>
+      <c r="F27" s="191"/>
+      <c r="G27" s="191"/>
+      <c r="H27" s="192"/>
       <c r="I27" s="28"/>
       <c r="J27" s="31"/>
-      <c r="K27" s="188">
+      <c r="K27" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L27" s="189"/>
-      <c r="M27" s="190"/>
-    </row>
-    <row r="28" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L27" s="184"/>
+      <c r="M27" s="185"/>
+    </row>
+    <row r="28" spans="1:13" ht="23" customHeight="1">
       <c r="A28" s="27"/>
-      <c r="B28" s="195"/>
-      <c r="C28" s="196"/>
-      <c r="D28" s="196"/>
-      <c r="E28" s="196"/>
-      <c r="F28" s="196"/>
-      <c r="G28" s="196"/>
-      <c r="H28" s="197"/>
+      <c r="B28" s="190"/>
+      <c r="C28" s="191"/>
+      <c r="D28" s="191"/>
+      <c r="E28" s="191"/>
+      <c r="F28" s="191"/>
+      <c r="G28" s="191"/>
+      <c r="H28" s="192"/>
       <c r="I28" s="28"/>
       <c r="J28" s="31"/>
-      <c r="K28" s="188">
+      <c r="K28" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L28" s="189"/>
-      <c r="M28" s="190"/>
-    </row>
-    <row r="29" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L28" s="184"/>
+      <c r="M28" s="185"/>
+    </row>
+    <row r="29" spans="1:13" ht="23" customHeight="1">
       <c r="A29" s="27"/>
-      <c r="B29" s="195"/>
-      <c r="C29" s="196"/>
-      <c r="D29" s="196"/>
-      <c r="E29" s="196"/>
-      <c r="F29" s="196"/>
-      <c r="G29" s="196"/>
-      <c r="H29" s="197"/>
+      <c r="B29" s="190"/>
+      <c r="C29" s="191"/>
+      <c r="D29" s="191"/>
+      <c r="E29" s="191"/>
+      <c r="F29" s="191"/>
+      <c r="G29" s="191"/>
+      <c r="H29" s="192"/>
       <c r="I29" s="28"/>
       <c r="J29" s="31"/>
-      <c r="K29" s="188">
+      <c r="K29" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L29" s="189"/>
-      <c r="M29" s="190"/>
-    </row>
-    <row r="30" spans="1:13" ht="23.1" customHeight="1">
+      <c r="L29" s="184"/>
+      <c r="M29" s="185"/>
+    </row>
+    <row r="30" spans="1:13" ht="23" customHeight="1">
       <c r="A30" s="27"/>
-      <c r="B30" s="195"/>
-      <c r="C30" s="196"/>
-      <c r="D30" s="196"/>
-      <c r="E30" s="196"/>
-      <c r="F30" s="196"/>
-      <c r="G30" s="196"/>
-      <c r="H30" s="197"/>
+      <c r="B30" s="190"/>
+      <c r="C30" s="191"/>
+      <c r="D30" s="191"/>
+      <c r="E30" s="191"/>
+      <c r="F30" s="191"/>
+      <c r="G30" s="191"/>
+      <c r="H30" s="192"/>
       <c r="I30" s="28"/>
       <c r="J30" s="31"/>
-      <c r="K30" s="188">
+      <c r="K30" s="183">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L30" s="189"/>
-      <c r="M30" s="190"/>
+      <c r="L30" s="184"/>
+      <c r="M30" s="185"/>
     </row>
     <row r="31" spans="1:13" ht="22.5" customHeight="1">
       <c r="J31" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K31" s="201">
+      <c r="K31" s="196">
         <f>SUM(K6:M30)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="202"/>
-      <c r="M31" s="203"/>
+      <c r="L31" s="197"/>
+      <c r="M31" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="56">
@@ -3828,5 +3873,10 @@
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.53" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>